<commit_message>
small adjustments + beri auto attack
</commit_message>
<xml_diff>
--- a/desert_fortresses.xlsx
+++ b/desert_fortresses.xlsx
@@ -314,7 +314,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -324,325 +324,397 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="n">
-        <v>282</v>
+        <v>243</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>243</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>09:27:35</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="n">
+        <v>282</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>243</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>14:47:35</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>360</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>243</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>09:23:50</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="n">
-        <v>282</v>
+        <v>399</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>243</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>10:32:06</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>45</v>
+        <v>56</v>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>10:42:55</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="n">
-        <v>282</v>
+        <v>380</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>14</v>
+        <v>54</v>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>02:07:37</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="n">
-        <v>360</v>
+        <v>419</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>02:07:16</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="n">
-        <v>438</v>
+        <v>458</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>10:33:39</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="n">
-        <v>282</v>
+        <v>497</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>10:33:25</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="n">
-        <v>321</v>
+        <v>536</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>49</v>
+        <v>58</v>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>04:27:18</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="n">
-        <v>360</v>
+        <v>575</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>34</v>
+        <v>25</v>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>03:41:54</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="n">
-        <v>399</v>
+        <v>614</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D12" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E12" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <v>16</v>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>03:12:14</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="n">
-        <v>438</v>
+        <v>653</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>13</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>50</v>
+        <v>57</v>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>15:18:44</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="n">
-        <v>477</v>
+        <v>731</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>13:55:50</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="n">
-        <v>243</v>
+        <v>809</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>02:34:55</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="n">
-        <v>282</v>
+        <v>926</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>16</v>
+        <v>38</v>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>17:06:16</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="n">
-        <v>243</v>
+        <v>965</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>14:28:40</t>
+          <t>17:36:59</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="0" t="n">
-        <v>282</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>243</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E18" s="0" t="n">
+      <c r="A18" t="n">
+        <v>1004</v>
+      </c>
+      <c r="B18" t="n">
+        <v>263</v>
+      </c>
+      <c r="C18" t="n">
+        <v>9</v>
+      </c>
+      <c r="D18" t="n">
         <v>39</v>
       </c>
-      <c r="F18" s="0" t="inlineStr">
-        <is>
-          <t>05:21:16</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0" t="n">
-        <v>360</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>243</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="F19" s="0" t="inlineStr">
-        <is>
-          <t>14:43:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>399</v>
-      </c>
-      <c r="B20" t="n">
-        <v>243</v>
-      </c>
-      <c r="C20" t="n">
-        <v>13</v>
-      </c>
-      <c r="D20" t="n">
-        <v>27</v>
-      </c>
-      <c r="E20" t="n">
-        <v>32</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>16:46:36</t>
+      <c r="E18" t="n">
+        <v>14</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>11:24:09</t>
         </is>
       </c>
     </row>

</xml_diff>